<commit_message>
Added Test Cases and standardizeEntityNames
Refined find/replace to only look for whole word
</commit_message>
<xml_diff>
--- a/tests/File_Util_TransformDD_Test.xlsx
+++ b/tests/File_Util_TransformDD_Test.xlsx
@@ -43,13 +43,13 @@
     <t>Agreement Packet ID</t>
   </si>
   <si>
+    <t>change word</t>
+  </si>
+  <si>
     <t>cas number</t>
   </si>
   <si>
     <t>CAS Number</t>
-  </si>
-  <si>
-    <t>change word</t>
   </si>
   <si>
     <t>uom</t>
@@ -366,8 +366,8 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -380,22 +380,22 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -409,7 +409,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>